<commit_message>
Localized sheets names in ユーザー.xlsx
</commit_message>
<xml_diff>
--- a/Config/JA/ユーザー.xlsx
+++ b/Config/JA/ユーザー.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus\Documents\GitHub\OrchestratorManager\Config\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02192CC4-6303-4449-8723-B729DF652D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD4F3B6-87D7-4E30-8B86-591911E05223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Get" sheetId="4" r:id="rId1"/>
-    <sheet name="Create" sheetId="1" r:id="rId2"/>
-    <sheet name="Edit" sheetId="5" r:id="rId3"/>
-    <sheet name="Delete" sheetId="2" r:id="rId4"/>
+    <sheet name="取得" sheetId="4" r:id="rId1"/>
+    <sheet name="作成" sheetId="1" r:id="rId2"/>
+    <sheet name="編集" sheetId="5" r:id="rId3"/>
+    <sheet name="削除" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>